<commit_message>
added GZGU statistics docs
</commit_message>
<xml_diff>
--- a/Statistics/InternalStatistics/Внутренняя_отчетность_комментарии расчета.xlsx
+++ b/Statistics/InternalStatistics/Внутренняя_отчетность_комментарии расчета.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18827"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Boris\Desktop\Проект_17\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Boris\Documents\GitHub\AdmissionOfficeStatistics\Statistics\InternalStatistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11145" tabRatio="854"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11145" tabRatio="854" firstSheet="2" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="1_Обобщенная по приему" sheetId="1" r:id="rId1"/>
@@ -21,8 +21,7 @@
     <sheet name="7_Анкета_целевики" sheetId="7" r:id="rId7"/>
     <sheet name="8_Анкета_проход.балл" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -175,58 +174,6 @@
     <t>!!!</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">!!! </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Механизм расчета здесь следующий:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>• Все пары Специальность-Форма обучения мы можем получить из результата слияния таблиц Speciality, KindLearn и PlanPr по соответствующим внешним ключам (см. описание таблиц).
-• Для каждой пары такого результата по парам идентификаторов мы будем выполнять подзапросы в таблице AbitSp, а именно, всего будет 3 группы подзапросов (в соответствии с нужными показателями): план приема, подано заявлений и зачислено. О том, как подсчитать каждый конкретный показать – см. выше в самой таблице.</t>
-    </r>
-  </si>
-  <si>
     <t>Берется из слияния таблицы Speciality, KindLearn и PlanPr, расчитывается как сумма Qo для тех строк, у которых форма обучения совпадает с текущей по идентификатору И специальность совпадает по имени Sp_Name с текущей, а поле Sp_C пустое (NULL)</t>
   </si>
   <si>
@@ -484,6 +431,69 @@
     <t>платно</t>
   </si>
   <si>
+    <t>пока не расчитывается, потому что не сошлись во мнении, как же корректнее посчитать этот показатель (олимпиадники бывают разные =)</t>
+  </si>
+  <si>
+    <t>Количество строк из слияния таблиц Speciality, KindLearn, AbitSp и Abit у которых форма обучения совпадает с текущей по идентификатору И специальность совпадает по имени Sp_Name с текущей И значение поля f=1 И Gr не Российская Федерация</t>
+  </si>
+  <si>
+    <t>не рассчитывается</t>
+  </si>
+  <si>
+    <t>Количество строк из слияния таблиц Speciality, KindLearn и AbitSp, у которых форма обучения совпадает с текущей по идентификатору И специальность совпадает по имени Sp_Name с текущей И значение поля f=1 И для которых существует строка в (слияние таблиц AbitInd и Ind_Documents, в которых идентификатор абитуриента aid совпадает с текущим, а наименование ИД ind_name включается в себя "медаль" или "диплом")</t>
+  </si>
+  <si>
+    <t>Количество строк из слияния таблиц Speciality, KindLearn, AbitSp и Abit у которых форма обучения совпадает с текущей по идентификатору И специальность совпадает по имени Sp_Name с текущей И значение поля f=1 И Gr Российская Федерация И Region не равен "Нижегородская область"</t>
+  </si>
+  <si>
+    <t>Количество строк из слияния таблиц Speciality, KindLearn, AbitSp и Abit у которых форма обучения совпадает с текущей по идентификатору И специальность совпадает по имени Sp_Name с текущей И значение поля f=1 И Gr Российская Федерация И Region "Нижегородская область"</t>
+  </si>
+  <si>
+    <t>Количество строк из слияния таблиц Speciality, KindLearn, AbitSp и Abit и Level_edu у которых форма обучения совпадает с текущей по идентификатору И специальность совпадает по имени Sp_Name с текущей И значение поля f=1 И S_Y = текущий год И наименование уровня образования leName включает в себя "среднее общее"</t>
+  </si>
+  <si>
+    <t>Количество строк из слияния таблиц Speciality, KindLearn, AbitSp и Abit и Level_edu у которых форма обучения совпадает с текущей по идентификатору И специальность совпадает по имени Sp_Name с текущей И значение поля f=1 И S_Y &lt; текущий год И наименование уровня образования leName включает в себя "среднее общее"</t>
+  </si>
+  <si>
+    <t>Количество строк из слияния таблиц Speciality, KindLearn, AbitSp и Abit и Level_edu у которых форма обучения совпадает с текущей по идентификатору И специальность совпадает по имени Sp_Name с текущей И значение поля f=1 И S_Y = текущий год И наименование уровня образования leName включает в себя "среднее профессиональное"</t>
+  </si>
+  <si>
+    <t>Количество строк из слияния таблиц Speciality, KindLearn, AbitSp и Abit и Level_edu у которых форма обучения совпадает с текущей по идентификатору И специальность совпадает по имени Sp_Name с текущей И значение поля f=1 И S_Y &lt; текущий год И наименование уровня образования leName включает в себя "среднее профессиональное"</t>
+  </si>
+  <si>
+    <t>Количество строк из таблицы AbitSp,где специальность и форма обучения совпадают с текущими по идентификаторам sp_id и kl_id, для которых не существует строк в таблице AbitEGE, у которых такой же идентификатор абитуриента aid И (какое-либо из полей d_ex gr заполнено (не равно NULL или пустой сроке))</t>
+  </si>
+  <si>
+    <t>Количество строк из таблицы AbitSp,где специальность и форма обучения совпадают с текущими по идентификаторам sp_id и kl_id, для которых существует хотя бы одна строка в таблице AbitEGE, у которой такой же идентификатор абитуриента aid И (какое-либо из полей d_ex gr заполнено (не равно NULL или пустой сроке))</t>
+  </si>
+  <si>
+    <t>Количество строк из слияния таблиц AbitSp, Abit и Level_edu, где специальность и форма обучения совпадают с текущими по идентификаторам sp_id и kl_id, для которых наименование уровня образования leName содержит слово "высшее"</t>
+  </si>
+  <si>
+    <t>Количество строк из слияния таблиц AbitSp, Abit и Level_edu, где специальность и форма обучения совпадают с текущими по идентификаторам sp_id и kl_id, для которых наименование уровня образования leName содержит слово "среднее"</t>
+  </si>
+  <si>
+    <t>Количество строк из таблицы AbitSp,у которых форма обучения совпадает с текущей по идентификатору И специальность совпадает по имени Sp_Name с текущей, для которых существует хотя бы одна строка в таблице AbitEGE, у которой такой же идентификатор абитуриента aid И (какое-либо из полей d_ex gr заполнено (не равно NULL или пустой сроке))</t>
+  </si>
+  <si>
+    <t>Как в Подано заявление + условие зачисления №8</t>
+  </si>
+  <si>
+    <t>Рассчитывается как среднее значение поля minb таблицы AbitSp, где  форма обучения совпадает с текущей по идентификатору И специальность совпадает по имени Sp_Name с текущей И значение поля f=1 И условие зачисления №8</t>
+  </si>
+  <si>
+    <t>В Платной форме все абсолютно так же, как в бюджете. Единственное, что меняется - это в Подано заяслений вместо условия f=1 становится условие f=2; а в Зачислено добавляется условие зачисления №9 вместо №8</t>
+  </si>
+  <si>
+    <t>*На самом деле, эта форма - это часть отчетной формы (1_Обобщенная по приему), но немного в другой перспективе. Но показатели идентичны, поэтому реализовав их для первой формы, в эту можно просто перенести нужные подзапросы</t>
+  </si>
+  <si>
+    <t>Количество строк из слияния таблиц AbitSp, Speciality, AbitAddInfo, AbitEGE, для которых уровень образования совпадает по идентификатору с текущим И специальность по названию совпадает с текущей И идентификатор предмета совпадает с текущим И отметка m100b &gt; 0</t>
+  </si>
+  <si>
+    <t>Количество строк в слиянии таблиц Speciality, AbitSp и Abit, для которых специальность по имени совпадает с текущей, форма обучения совпадает с текущей по идентификатору, поле льготы l1_id = идентификатору текущей категории квоты</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -531,63 +541,24 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>• Все пары Специальность-Форма обучения мы можем получить из результата слияния таблиц Speciality, KindLearn и PlanPr по соответствующим внешним ключам (см. описание таблиц).
-• Для каждой пары такого результата по парам идентификаторов мы будем выполнять подзапросы в таблице AbitSp сначала для бюджета (дополнительное условие f=1), затем для платной формы (дополнительное услвоие f=2), а именно, всего будет 2 группы подзапросов (в соответствии с нужными показателями): подано заявлений и зачислено. О том, как подсчитать каждый конкретный показать – см. выше в самой таблице.</t>
-    </r>
-  </si>
-  <si>
-    <t>пока не расчитывается, потому что не сошлись во мнении, как же корректнее посчитать этот показатель (олимпиадники бывают разные =)</t>
-  </si>
-  <si>
-    <t>Количество строк из слияния таблиц Speciality, KindLearn, AbitSp и Abit у которых форма обучения совпадает с текущей по идентификатору И специальность совпадает по имени Sp_Name с текущей И значение поля f=1 И Gr не Российская Федерация</t>
-  </si>
-  <si>
-    <t>не рассчитывается</t>
-  </si>
-  <si>
-    <t>Количество строк из слияния таблиц Speciality, KindLearn и AbitSp, у которых форма обучения совпадает с текущей по идентификатору И специальность совпадает по имени Sp_Name с текущей И значение поля f=1 И для которых существует строка в (слияние таблиц AbitInd и Ind_Documents, в которых идентификатор абитуриента aid совпадает с текущим, а наименование ИД ind_name включается в себя "медаль" или "диплом")</t>
-  </si>
-  <si>
-    <t>Количество строк из слияния таблиц Speciality, KindLearn, AbitSp и Abit у которых форма обучения совпадает с текущей по идентификатору И специальность совпадает по имени Sp_Name с текущей И значение поля f=1 И Gr Российская Федерация И Region не равен "Нижегородская область"</t>
-  </si>
-  <si>
-    <t>Количество строк из слияния таблиц Speciality, KindLearn, AbitSp и Abit у которых форма обучения совпадает с текущей по идентификатору И специальность совпадает по имени Sp_Name с текущей И значение поля f=1 И Gr Российская Федерация И Region "Нижегородская область"</t>
-  </si>
-  <si>
-    <t>Количество строк из слияния таблиц Speciality, KindLearn, AbitSp и Abit и Level_edu у которых форма обучения совпадает с текущей по идентификатору И специальность совпадает по имени Sp_Name с текущей И значение поля f=1 И S_Y = текущий год И наименование уровня образования leName включает в себя "среднее общее"</t>
-  </si>
-  <si>
-    <t>Количество строк из слияния таблиц Speciality, KindLearn, AbitSp и Abit и Level_edu у которых форма обучения совпадает с текущей по идентификатору И специальность совпадает по имени Sp_Name с текущей И значение поля f=1 И S_Y &lt; текущий год И наименование уровня образования leName включает в себя "среднее общее"</t>
-  </si>
-  <si>
-    <t>Количество строк из слияния таблиц Speciality, KindLearn, AbitSp и Abit и Level_edu у которых форма обучения совпадает с текущей по идентификатору И специальность совпадает по имени Sp_Name с текущей И значение поля f=1 И S_Y = текущий год И наименование уровня образования leName включает в себя "среднее профессиональное"</t>
-  </si>
-  <si>
-    <t>Количество строк из слияния таблиц Speciality, KindLearn, AbitSp и Abit и Level_edu у которых форма обучения совпадает с текущей по идентификатору И специальность совпадает по имени Sp_Name с текущей И значение поля f=1 И S_Y &lt; текущий год И наименование уровня образования leName включает в себя "среднее профессиональное"</t>
-  </si>
-  <si>
-    <t>Количество строк из таблицы AbitSp,где специальность и форма обучения совпадают с текущими по идентификаторам sp_id и kl_id, для которых не существует строк в таблице AbitEGE, у которых такой же идентификатор абитуриента aid И (какое-либо из полей d_ex gr заполнено (не равно NULL или пустой сроке))</t>
-  </si>
-  <si>
-    <t>Количество строк из таблицы AbitSp,где специальность и форма обучения совпадают с текущими по идентификаторам sp_id и kl_id, для которых существует хотя бы одна строка в таблице AbitEGE, у которой такой же идентификатор абитуриента aid И (какое-либо из полей d_ex gr заполнено (не равно NULL или пустой сроке))</t>
-  </si>
-  <si>
-    <t>Количество строк из слияния таблиц AbitSp, Abit и Level_edu, где специальность и форма обучения совпадают с текущими по идентификаторам sp_id и kl_id, для которых наименование уровня образования leName содержит слово "высшее"</t>
-  </si>
-  <si>
-    <t>Количество строк из слияния таблиц AbitSp, Abit и Level_edu, где специальность и форма обучения совпадают с текущими по идентификаторам sp_id и kl_id, для которых наименование уровня образования leName содержит слово "среднее"</t>
-  </si>
-  <si>
-    <t>Количество строк из таблицы AbitSp,у которых форма обучения совпадает с текущей по идентификатору И специальность совпадает по имени Sp_Name с текущей, для которых существует хотя бы одна строка в таблице AbitEGE, у которой такой же идентификатор абитуриента aid И (какое-либо из полей d_ex gr заполнено (не равно NULL или пустой сроке))</t>
-  </si>
-  <si>
-    <t>Как в Подано заявление + условие зачисления №8</t>
-  </si>
-  <si>
-    <t>Рассчитывается как среднее значение поля minb таблицы AbitSp, где  форма обучения совпадает с текущей по идентификатору И специальность совпадает по имени Sp_Name с текущей И значение поля f=1 И условие зачисления №8</t>
-  </si>
-  <si>
-    <t>В Платной форме все абсолютно так же, как в бюджете. Единственное, что меняется - это в Подано заяслений вместо условия f=1 становится условие f=2; а в Зачислено добавляется условие зачисления №9 вместо №8</t>
+      <t>• Все пары Субъект-Специальность мы можем получить из декартова произведения таблиц Abit (поле Region) и Speciality. При этом проверяем для полученного результата, что существует хотя бы одна строка в слиянии таблиц Speciality с PlanPr, в котрой специальность по имени совпадает с текущей и sp_C содержит в себе текущий субъект.
+• Для каждого такого результата мы будем выполнять подзапросы. О том, как подсчитать каждый конкретный показать – см. выше в самой таблице.</t>
+    </r>
+  </si>
+  <si>
+    <t>Равен сумме значений Qo из слияния таблиц Speciality и PlanPr, где специальность совпадает с текущей по имени и sp_C содержит в себе текущий субъект.</t>
+  </si>
+  <si>
+    <t>Равен количеству строк в слиянии таблиц Speciality и AbitSp, где специальность совпадает с текущей по имени и sp_C содержит в себе текущий субъект.</t>
+  </si>
+  <si>
+    <t>Считается как минимум суммы полей (minb+ind_ball) из сляния таблиц Speciality и AbitSp, где специальность совпадает с текущей по имени и sp_C содержит в себе текущий субъект + условие зачисления №3</t>
+  </si>
+  <si>
+    <t>Считается как минимум суммы полей (minb+ind_ball) из сляния таблиц Speciality и AbitSp, где специальность совпадает с текущей по имени и идентификатор формы обучения равен текущему И f=1 + условие зачисления №8</t>
+  </si>
+  <si>
+    <t>Считается как минимум суммы полей (minb+ind_ball) из сляния таблиц Speciality и AbitSp, где специальность совпадает с текущей по имени и идентификатор формы обучения равен текущему И f=2 + условие зачисления №9</t>
   </si>
   <si>
     <r>
@@ -637,15 +608,9 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>• Все пары Специальность-Форма обучения мы можем получить из результата слияния таблиц Speciality, KindLearn и PlanPr по соответствующим внешним ключам (см. описание таблиц).
-• Для каждой пары такого результата по парам идентификаторов мы будем выполнять подзапросы в таблице AbitSp. О том, как подсчитать каждый конкретный показать – см. выше в самой таблице.</t>
-    </r>
-  </si>
-  <si>
-    <t>*На самом деле, эта форма - это часть отчетной формы (1_Обобщенная по приему), но немного в другой перспективе. Но показатели идентичны, поэтому реализовав их для первой формы, в эту можно просто перенести нужные подзапросы</t>
-  </si>
-  <si>
-    <t>Количество строк из слияния таблиц AbitSp, Speciality, AbitAddInfo, AbitEGE, для которых уровень образования совпадает по идентификатору с текущим И специальность по названию совпадает с текущей И идентификатор предмета совпадает с текущим И отметка m100b &gt; 0</t>
+      <t>• Все пары Специальность-Форма обучения мы можем получить из результата слияния таблиц Speciality, KindLearn и PlanPr по соответствующим внешним ключам (см. описание таблиц).Единственное ограничение здесь - нам нужны строки, где Sp_C пустое (NULL)
+• Для каждой пары такого результата по парам идентификаторов мы будем выполнять подзапросы в таблице AbitSp, а именно, всего будет 3 группы подзапросов (в соответствии с нужными показателями): план приема, подано заявлений и зачислено. О том, как подсчитать каждый конкретный показать – см. выше в самой таблице.</t>
+    </r>
   </si>
   <si>
     <r>
@@ -695,8 +660,8 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>• Все четверки Специальность-Форма обучения-Наименование олимпиады-Предмет мы можем получить из результата декартова произведения таблиц Speciality, KindLearn, AbitAddInfo, Exam. Но при этом надо наложить условие, что для четверки существует хотя бы одна строка в слиянии таблиц Speciality, AbitSp и AbitAddInfo (то есть, в этой строке идентификатор специальности равен текущей, наименование специальности равно текущему, наименование олимпиады равно текущему) - иначе говоря, что вообще у нас хотя бы один олимпиадник подавал документы.
-• Для каждой такого результата (иначе, для каждой четверки) мы будем выполнять подзапросы. О том, как подсчитать каждый конкретный показать – см. выше в самой таблице.</t>
+      <t>• Все пары Специальность-Форма обучения мы можем получить из результата слияния таблиц Speciality, KindLearn и PlanPr по соответствующим внешним ключам (см. описание таблиц).Единственное ограничение здесь - нам нужны строки, где Sp_C пустое (NULL)
+• Для каждой пары такого результата по парам идентификаторов мы будем выполнять подзапросы в таблице AbitSp сначала для бюджета (дополнительное условие f=1), затем для платной формы (дополнительное услвоие f=2), а именно, всего будет 2 группы подзапросов (в соответствии с нужными показателями): подано заявлений и зачислено. О том, как подсчитать каждый конкретный показать – см. выше в самой таблице.</t>
     </r>
   </si>
   <si>
@@ -747,12 +712,9 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>• Все тройки Специальность-Форма обучения-Категория квоты мы можем получить из декартова произведения таблиц Speciality, KindLearn и Lgot1.
-• Для каждого такого результата мы будем выполнять подзапросы в таблице AbitSp. О том, как подсчитать каждый конкретный показать – см. выше в самой таблице.</t>
-    </r>
-  </si>
-  <si>
-    <t>Количество строк в слиянии таблиц Speciality, AbitSp и Abit, для которых специальность по имени совпадает с текущей, форма обучения совпадает с текущей по идентификатору, поле льготы l1_id = идентификатору текущей категории квоты</t>
+      <t>• Все пары Специальность-Форма обучения мы можем получить из результата слияния таблиц Speciality, KindLearn и PlanPr по соответствующим внешним ключам (см. описание таблиц).Единственное ограничение здесь - нам нужны строки, где Sp_C пустое (NULL)
+• Для каждой пары такого результата по парам идентификаторов мы будем выполнять подзапросы в таблице AbitSp. О том, как подсчитать каждый конкретный показать – см. выше в самой таблице.</t>
+    </r>
   </si>
   <si>
     <r>
@@ -802,30 +764,67 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>• Все пары Субъект-Специальность мы можем получить из декартова произведения таблиц Abit (поле Region) и Speciality. При этом проверяем для полученного результата, что существует хотя бы одна строка в слиянии таблиц Speciality с PlanPr, в котрой специальность по имени совпадает с текущей и sp_C содержит в себе текущий субъект.
-• Для каждого такого результата мы будем выполнять подзапросы. О том, как подсчитать каждый конкретный показать – см. выше в самой таблице.</t>
-    </r>
-  </si>
-  <si>
-    <t>Равен сумме значений Qo из слияния таблиц Speciality и PlanPr, где специальность совпадает с текущей по имени и sp_C содержит в себе текущий субъект.</t>
-  </si>
-  <si>
-    <t>Равен количеству строк в слиянии таблиц Speciality и AbitSp, где специальность совпадает с текущей по имени и sp_C содержит в себе текущий субъект.</t>
-  </si>
-  <si>
-    <t>Считается как минимум суммы полей (minb+ind_ball) из сляния таблиц Speciality и AbitSp, где специальность совпадает с текущей по имени и sp_C содержит в себе текущий субъект + условие зачисления №3</t>
-  </si>
-  <si>
-    <t>Считается как минимум суммы полей (minb+ind_ball) из сляния таблиц Speciality и AbitSp, где специальность совпадает с текущей по имени и идентификатор формы обучения равен текущему И f=1 + условие зачисления №8</t>
-  </si>
-  <si>
-    <t>Считается как минимум суммы полей (minb+ind_ball) из сляния таблиц Speciality и AbitSp, где специальность совпадает с текущей по имени и идентификатор формы обучения равен текущему И f=2 + условие зачисления №9</t>
+      <t>• Все четверки Специальность-Форма обучения-Наименование олимпиады-Предмет мы можем получить из результата декартова произведения таблиц Speciality, KindLearn, AbitAddInfo, Exam. Но при этом надо наложить условие, что для четверки существует хотя бы одна строка в слиянии таблиц Speciality, AbitSp и AbitAddInfo (то есть, в этой строке идентификатор специальности равен текущей, наименование специальности равно текущему, наименование олимпиады равно текущему) - иначе говоря, что вообще у нас хотя бы один олимпиадник подавал документы.Единственное ограничение здесь - нам нужны строки, где Sp_C пустое (NULL)
+• Для каждой такого результата (иначе, для каждой четверки) мы будем выполнять подзапросы. О том, как подсчитать каждый конкретный показать – см. выше в самой таблице.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">!!! </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Механизм расчета здесь следующий:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>• Все тройки Специальность-Форма обучения-Категория квоты мы можем получить из декартова произведения таблиц Speciality, KindLearn и Lgot1.Единственное ограничение здесь - нам нужны строки, где Sp_C пустое (NULL)
+• Для каждого такого результата мы будем выполнять подзапросы в таблице AbitSp. О том, как подсчитать каждый конкретный показать – см. выше в самой таблице.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1521,6 +1520,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1557,6 +1565,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1614,8 +1625,11 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1670,21 +1684,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1968,8 +1967,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection sqref="A1:A2"/>
+    <sheetView topLeftCell="A4" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1992,37 +1991,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="D1" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="41" t="s">
+      <c r="E1" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="41"/>
-      <c r="M1" s="41"/>
-      <c r="N1" s="41"/>
-      <c r="O1" s="42"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
+      <c r="N1" s="44"/>
+      <c r="O1" s="45"/>
     </row>
     <row r="2" spans="1:15" s="6" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="47"/>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="44"/>
+      <c r="A2" s="50"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="47"/>
       <c r="E2" s="10" t="s">
         <v>5</v>
       </c>
@@ -2058,110 +2057,110 @@
       </c>
     </row>
     <row r="3" spans="1:15" s="22" customFormat="1" ht="240" x14ac:dyDescent="0.25">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="38"/>
+      <c r="B3" s="41"/>
       <c r="C3" s="26" t="s">
         <v>44</v>
       </c>
       <c r="D3" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="E3" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="F3" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="F3" s="25" t="s">
+      <c r="G3" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="G3" s="25" t="s">
-        <v>58</v>
-      </c>
       <c r="H3" s="25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I3" s="25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J3" s="24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K3" s="25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L3" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="M3" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="N3" s="25" t="s">
         <v>83</v>
       </c>
-      <c r="M3" s="25" t="s">
+      <c r="O3" s="25" t="s">
         <v>84</v>
       </c>
-      <c r="N3" s="25" t="s">
-        <v>85</v>
-      </c>
-      <c r="O3" s="25" t="s">
-        <v>86</v>
-      </c>
     </row>
     <row r="4" spans="1:15" s="22" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="39"/>
-      <c r="B4" s="39"/>
+      <c r="A4" s="42"/>
+      <c r="B4" s="42"/>
       <c r="C4" s="23" t="s">
         <v>45</v>
       </c>
       <c r="D4" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="E4" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="F4" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="F4" s="24" t="s">
+      <c r="G4" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="G4" s="24" t="s">
+      <c r="H4" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="H4" s="24" t="s">
+      <c r="I4" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="I4" s="24" t="s">
-        <v>65</v>
-      </c>
       <c r="J4" s="24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K4" s="24" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L4" s="24" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M4" s="24" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="N4" s="24" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="O4" s="24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:15" s="22" customFormat="1" ht="150" x14ac:dyDescent="0.25">
-      <c r="A5" s="39"/>
-      <c r="B5" s="39"/>
+      <c r="A5" s="42"/>
+      <c r="B5" s="42"/>
       <c r="C5" s="23" t="s">
         <v>16</v>
       </c>
       <c r="D5" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="E5" s="25" t="s">
+      <c r="F5" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="F5" s="25" t="s">
-        <v>53</v>
-      </c>
       <c r="G5" s="25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H5" s="27"/>
       <c r="I5" s="28"/>
@@ -2173,17 +2172,17 @@
       <c r="O5" s="27"/>
     </row>
     <row r="8" spans="1:15" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="B8" s="40"/>
-      <c r="C8" s="40"/>
-      <c r="D8" s="40"/>
-      <c r="E8" s="40"/>
-      <c r="F8" s="40"/>
-      <c r="G8" s="40"/>
-      <c r="H8" s="40"/>
-      <c r="I8" s="40"/>
+      <c r="A8" s="43" t="s">
+        <v>98</v>
+      </c>
+      <c r="B8" s="43"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="43"/>
+      <c r="I8" s="43"/>
       <c r="J8" s="20"/>
       <c r="K8" s="20"/>
       <c r="L8" s="20"/>
@@ -2191,17 +2190,17 @@
       <c r="N8" s="20"/>
     </row>
     <row r="10" spans="1:15" ht="217.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="40" t="s">
-        <v>59</v>
-      </c>
-      <c r="B10" s="40"/>
-      <c r="C10" s="40"/>
-      <c r="D10" s="40"/>
-      <c r="E10" s="40"/>
-      <c r="F10" s="40"/>
-      <c r="G10" s="40"/>
-      <c r="H10" s="40"/>
-      <c r="I10" s="40"/>
+      <c r="A10" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="43"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="43"/>
+      <c r="H10" s="43"/>
+      <c r="I10" s="43"/>
       <c r="J10" s="20"/>
     </row>
   </sheetData>
@@ -2249,42 +2248,42 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="51" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="48"/>
+      <c r="B2" s="51"/>
       <c r="C2" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="D2" s="24" t="s">
-        <v>70</v>
-      </c>
     </row>
     <row r="7" spans="1:9" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="40" t="s">
-        <v>68</v>
-      </c>
-      <c r="B7" s="40"/>
-      <c r="C7" s="40"/>
-      <c r="D7" s="40"/>
-      <c r="E7" s="40"/>
-      <c r="F7" s="40"/>
-      <c r="G7" s="40"/>
-      <c r="H7" s="40"/>
-      <c r="I7" s="40"/>
+      <c r="A7" s="43" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="43"/>
+      <c r="C7" s="43"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="43"/>
     </row>
     <row r="10" spans="1:9" ht="216" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="40" t="s">
-        <v>59</v>
-      </c>
-      <c r="B10" s="40"/>
-      <c r="C10" s="40"/>
-      <c r="D10" s="40"/>
-      <c r="E10" s="40"/>
-      <c r="F10" s="40"/>
-      <c r="G10" s="40"/>
-      <c r="H10" s="40"/>
-      <c r="I10" s="40"/>
+      <c r="A10" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="43"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="43"/>
+      <c r="H10" s="43"/>
+      <c r="I10" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2302,7 +2301,7 @@
   <dimension ref="A1:Q12"/>
   <sheetViews>
     <sheetView zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2327,42 +2326,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="D1" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="43" t="s">
+      <c r="E1" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="F1" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="41"/>
-      <c r="M1" s="41"/>
-      <c r="N1" s="41"/>
-      <c r="O1" s="41"/>
-      <c r="P1" s="68"/>
-      <c r="Q1" s="42"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
+      <c r="N1" s="44"/>
+      <c r="O1" s="44"/>
+      <c r="P1" s="52"/>
+      <c r="Q1" s="45"/>
     </row>
     <row r="2" spans="1:17" s="6" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="47"/>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="44"/>
+      <c r="A2" s="50"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="47"/>
       <c r="F2" s="10" t="s">
         <v>22</v>
       </c>
@@ -2401,142 +2400,142 @@
       </c>
     </row>
     <row r="3" spans="1:17" s="22" customFormat="1" ht="255" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="62" t="s">
+      <c r="A3" s="66" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="63"/>
-      <c r="C3" s="59" t="s">
+      <c r="B3" s="67"/>
+      <c r="C3" s="63" t="s">
         <v>21</v>
       </c>
       <c r="D3" s="30" t="s">
         <v>44</v>
       </c>
       <c r="E3" s="31" t="s">
-        <v>56</v>
-      </c>
-      <c r="F3" s="49" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" s="53" t="s">
+        <v>71</v>
+      </c>
+      <c r="G3" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="H3" s="53" t="s">
         <v>73</v>
       </c>
-      <c r="G3" s="34" t="s">
+      <c r="I3" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="H3" s="49" t="s">
+      <c r="J3" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="K3" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="I3" s="34" t="s">
-        <v>76</v>
-      </c>
-      <c r="J3" s="34" t="s">
+      <c r="L3" s="34" t="s">
+        <v>77</v>
+      </c>
+      <c r="M3" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="K3" s="34" t="s">
-        <v>77</v>
-      </c>
-      <c r="L3" s="34" t="s">
+      <c r="N3" s="34" t="s">
         <v>79</v>
       </c>
-      <c r="M3" s="34" t="s">
+      <c r="O3" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="N3" s="34" t="s">
-        <v>81</v>
-      </c>
-      <c r="O3" s="34" t="s">
-        <v>82</v>
-      </c>
       <c r="P3" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q3" s="61" t="s">
         <v>87</v>
       </c>
-      <c r="Q3" s="57" t="s">
-        <v>89</v>
-      </c>
     </row>
     <row r="4" spans="1:17" s="22" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="64"/>
-      <c r="B4" s="65"/>
-      <c r="C4" s="60"/>
+      <c r="A4" s="68"/>
+      <c r="B4" s="69"/>
+      <c r="C4" s="64"/>
       <c r="D4" s="35" t="s">
         <v>45</v>
       </c>
       <c r="E4" s="36" t="s">
-        <v>88</v>
-      </c>
-      <c r="F4" s="50"/>
+        <v>86</v>
+      </c>
+      <c r="F4" s="54"/>
       <c r="G4" s="36" t="s">
-        <v>88</v>
-      </c>
-      <c r="H4" s="50"/>
+        <v>86</v>
+      </c>
+      <c r="H4" s="54"/>
       <c r="I4" s="36" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="J4" s="36" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="K4" s="36" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="L4" s="36" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="M4" s="36" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="N4" s="36" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="O4" s="36" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="P4" s="36" t="s">
-        <v>88</v>
-      </c>
-      <c r="Q4" s="58"/>
+        <v>86</v>
+      </c>
+      <c r="Q4" s="62"/>
     </row>
     <row r="5" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="64"/>
-      <c r="B5" s="65"/>
-      <c r="C5" s="59" t="s">
-        <v>71</v>
+      <c r="A5" s="68"/>
+      <c r="B5" s="69"/>
+      <c r="C5" s="63" t="s">
+        <v>70</v>
       </c>
       <c r="D5" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="E5" s="51" t="s">
-        <v>90</v>
-      </c>
-      <c r="F5" s="52"/>
-      <c r="G5" s="52"/>
-      <c r="H5" s="52"/>
-      <c r="I5" s="52"/>
-      <c r="J5" s="52"/>
-      <c r="K5" s="52"/>
-      <c r="L5" s="52"/>
-      <c r="M5" s="52"/>
-      <c r="N5" s="52"/>
-      <c r="O5" s="52"/>
-      <c r="P5" s="52"/>
-      <c r="Q5" s="53"/>
+      <c r="E5" s="55" t="s">
+        <v>88</v>
+      </c>
+      <c r="F5" s="56"/>
+      <c r="G5" s="56"/>
+      <c r="H5" s="56"/>
+      <c r="I5" s="56"/>
+      <c r="J5" s="56"/>
+      <c r="K5" s="56"/>
+      <c r="L5" s="56"/>
+      <c r="M5" s="56"/>
+      <c r="N5" s="56"/>
+      <c r="O5" s="56"/>
+      <c r="P5" s="56"/>
+      <c r="Q5" s="57"/>
     </row>
     <row r="6" spans="1:17" s="22" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="66"/>
-      <c r="B6" s="67"/>
-      <c r="C6" s="61"/>
+      <c r="A6" s="70"/>
+      <c r="B6" s="71"/>
+      <c r="C6" s="65"/>
       <c r="D6" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="E6" s="54"/>
-      <c r="F6" s="55"/>
-      <c r="G6" s="55"/>
-      <c r="H6" s="55"/>
-      <c r="I6" s="55"/>
-      <c r="J6" s="55"/>
-      <c r="K6" s="55"/>
-      <c r="L6" s="55"/>
-      <c r="M6" s="55"/>
-      <c r="N6" s="55"/>
-      <c r="O6" s="55"/>
-      <c r="P6" s="55"/>
-      <c r="Q6" s="56"/>
+      <c r="E6" s="58"/>
+      <c r="F6" s="59"/>
+      <c r="G6" s="59"/>
+      <c r="H6" s="59"/>
+      <c r="I6" s="59"/>
+      <c r="J6" s="59"/>
+      <c r="K6" s="59"/>
+      <c r="L6" s="59"/>
+      <c r="M6" s="59"/>
+      <c r="N6" s="59"/>
+      <c r="O6" s="59"/>
+      <c r="P6" s="59"/>
+      <c r="Q6" s="60"/>
     </row>
     <row r="7" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20"/>
@@ -2558,39 +2557,33 @@
       <c r="Q7" s="21"/>
     </row>
     <row r="9" spans="1:17" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="40" t="s">
-        <v>72</v>
-      </c>
-      <c r="B9" s="40"/>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="40"/>
-      <c r="G9" s="40"/>
-      <c r="H9" s="40"/>
-      <c r="I9" s="40"/>
+      <c r="A9" s="43" t="s">
+        <v>99</v>
+      </c>
+      <c r="B9" s="43"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="43"/>
+      <c r="I9" s="43"/>
     </row>
     <row r="12" spans="1:17" ht="218.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="40" t="s">
-        <v>59</v>
-      </c>
-      <c r="B12" s="40"/>
-      <c r="C12" s="40"/>
-      <c r="D12" s="40"/>
-      <c r="E12" s="40"/>
-      <c r="F12" s="40"/>
-      <c r="G12" s="40"/>
-      <c r="H12" s="40"/>
-      <c r="I12" s="40"/>
+      <c r="A12" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" s="43"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="43"/>
+      <c r="I12" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="F1:Q1"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
     <mergeCell ref="A12:I12"/>
     <mergeCell ref="F3:F4"/>
     <mergeCell ref="H3:H4"/>
@@ -2600,6 +2593,12 @@
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="A3:B6"/>
+    <mergeCell ref="F1:Q1"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2610,7 +2609,7 @@
   <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD10"/>
+      <selection sqref="A1:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2633,181 +2632,175 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="68" t="s">
+      <c r="C1" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="80"/>
-      <c r="G1" s="68" t="s">
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="71"/>
-      <c r="I1" s="71"/>
-      <c r="J1" s="80"/>
-      <c r="K1" s="68" t="s">
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="85"/>
+      <c r="K1" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="L1" s="71"/>
-      <c r="M1" s="71"/>
-      <c r="N1" s="72"/>
+      <c r="L1" s="76"/>
+      <c r="M1" s="76"/>
+      <c r="N1" s="77"/>
     </row>
     <row r="2" spans="1:14" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="69"/>
-      <c r="B2" s="70"/>
-      <c r="C2" s="73" t="s">
+      <c r="A2" s="74"/>
+      <c r="B2" s="75"/>
+      <c r="C2" s="78" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="75" t="s">
+      <c r="D2" s="80" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="75"/>
-      <c r="F2" s="78" t="s">
+      <c r="E2" s="80"/>
+      <c r="F2" s="83" t="s">
         <v>36</v>
       </c>
-      <c r="G2" s="73" t="s">
+      <c r="G2" s="78" t="s">
         <v>37</v>
       </c>
-      <c r="H2" s="75" t="s">
+      <c r="H2" s="80" t="s">
         <v>34</v>
       </c>
-      <c r="I2" s="75"/>
-      <c r="J2" s="78" t="s">
+      <c r="I2" s="80"/>
+      <c r="J2" s="83" t="s">
         <v>36</v>
       </c>
-      <c r="K2" s="73" t="s">
+      <c r="K2" s="78" t="s">
         <v>37</v>
       </c>
-      <c r="L2" s="75" t="s">
+      <c r="L2" s="80" t="s">
         <v>34</v>
       </c>
-      <c r="M2" s="75"/>
-      <c r="N2" s="76" t="s">
+      <c r="M2" s="80"/>
+      <c r="N2" s="81" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:14" s="6" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="47"/>
-      <c r="B3" s="45"/>
-      <c r="C3" s="74"/>
+      <c r="A3" s="50"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="79"/>
       <c r="D3" s="16" t="s">
         <v>3</v>
       </c>
       <c r="E3" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="F3" s="79"/>
-      <c r="G3" s="74"/>
+      <c r="F3" s="84"/>
+      <c r="G3" s="79"/>
       <c r="H3" s="16" t="s">
         <v>3</v>
       </c>
       <c r="I3" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="J3" s="79"/>
-      <c r="K3" s="74"/>
+      <c r="J3" s="84"/>
+      <c r="K3" s="79"/>
       <c r="L3" s="16" t="s">
         <v>3</v>
       </c>
       <c r="M3" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="N3" s="77"/>
+      <c r="N3" s="82"/>
     </row>
     <row r="4" spans="1:14" ht="165" x14ac:dyDescent="0.25">
-      <c r="A4" s="87" t="s">
+      <c r="A4" s="72" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="88"/>
+      <c r="B4" s="73"/>
       <c r="C4" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="E4" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="E4" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="F4" s="25" t="s">
-        <v>53</v>
-      </c>
       <c r="G4" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="H4" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="H4" s="25" t="s">
+      <c r="I4" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="J4" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="I4" s="25" t="s">
+      <c r="K4" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="L4" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="M4" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="N4" s="24" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="43" t="s">
+        <v>89</v>
+      </c>
+      <c r="B6" s="43"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+    </row>
+    <row r="8" spans="1:14" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="43" t="s">
+        <v>100</v>
+      </c>
+      <c r="B8" s="43"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="43"/>
+      <c r="I8" s="43"/>
+    </row>
+    <row r="10" spans="1:14" ht="219.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="43" t="s">
         <v>58</v>
       </c>
-      <c r="J4" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="K4" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="L4" s="24" t="s">
-        <v>61</v>
-      </c>
-      <c r="M4" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="N4" s="24" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="40" t="s">
-        <v>92</v>
-      </c>
-      <c r="B6" s="40"/>
-      <c r="C6" s="40"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="40"/>
-      <c r="H6" s="40"/>
-    </row>
-    <row r="8" spans="1:14" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="B8" s="40"/>
-      <c r="C8" s="40"/>
-      <c r="D8" s="40"/>
-      <c r="E8" s="40"/>
-      <c r="F8" s="40"/>
-      <c r="G8" s="40"/>
-      <c r="H8" s="40"/>
-      <c r="I8" s="40"/>
-    </row>
-    <row r="10" spans="1:14" ht="219.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="40" t="s">
-        <v>59</v>
-      </c>
-      <c r="B10" s="40"/>
-      <c r="C10" s="40"/>
-      <c r="D10" s="40"/>
-      <c r="E10" s="40"/>
-      <c r="F10" s="40"/>
-      <c r="G10" s="40"/>
-      <c r="H10" s="40"/>
-      <c r="I10" s="40"/>
+      <c r="B10" s="43"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="43"/>
+      <c r="H10" s="43"/>
+      <c r="I10" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A10:I10"/>
-    <mergeCell ref="A6:H6"/>
-    <mergeCell ref="A8:I8"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:B3"/>
     <mergeCell ref="K1:N1"/>
     <mergeCell ref="K2:K3"/>
     <mergeCell ref="L2:M2"/>
@@ -2820,6 +2813,12 @@
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="G1:J1"/>
     <mergeCell ref="J2:J3"/>
+    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="A6:H6"/>
+    <mergeCell ref="A8:I8"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2830,7 +2829,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2844,59 +2843,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="3" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="81" t="s">
+      <c r="C1" s="86" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="81" t="s">
+      <c r="D1" s="86" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="81" t="s">
+      <c r="E1" s="86" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="83" t="s">
+      <c r="F1" s="88" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="47"/>
-      <c r="B2" s="45"/>
-      <c r="C2" s="82"/>
-      <c r="D2" s="82"/>
-      <c r="E2" s="82"/>
-      <c r="F2" s="84"/>
+      <c r="A2" s="50"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="87"/>
+      <c r="D2" s="87"/>
+      <c r="E2" s="87"/>
+      <c r="F2" s="89"/>
     </row>
     <row r="3" spans="1:9" ht="150" x14ac:dyDescent="0.25">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="51" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="48"/>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="89" t="s">
-        <v>93</v>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="37" t="s">
+        <v>90</v>
       </c>
       <c r="F3" s="36" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="40" t="s">
-        <v>94</v>
-      </c>
-      <c r="B11" s="40"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="40"/>
+      <c r="A11" s="43" t="s">
+        <v>101</v>
+      </c>
+      <c r="B11" s="43"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="43"/>
     </row>
     <row r="12" spans="1:9" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="4"/>
@@ -2908,17 +2907,17 @@
       <c r="I12" s="5"/>
     </row>
     <row r="13" spans="1:9" ht="234" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="40" t="s">
-        <v>59</v>
-      </c>
-      <c r="B13" s="40"/>
-      <c r="C13" s="40"/>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="40"/>
+      <c r="A13" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" s="43"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="43"/>
+      <c r="I13" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -2941,7 +2940,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2954,54 +2953,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="81" t="s">
+      <c r="C1" s="86" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="81" t="s">
+      <c r="D1" s="86" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="83" t="s">
+      <c r="E1" s="88" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="47"/>
-      <c r="B2" s="45"/>
-      <c r="C2" s="82"/>
-      <c r="D2" s="82"/>
-      <c r="E2" s="84"/>
+      <c r="A2" s="50"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="87"/>
+      <c r="D2" s="87"/>
+      <c r="E2" s="89"/>
     </row>
     <row r="3" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A3" s="87" t="s">
+      <c r="A3" s="72" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="87"/>
-      <c r="C3" s="88"/>
-      <c r="D3" s="90" t="s">
-        <v>96</v>
-      </c>
-      <c r="E3" s="91" t="s">
-        <v>60</v>
+      <c r="B3" s="72"/>
+      <c r="C3" s="73"/>
+      <c r="D3" s="38" t="s">
+        <v>91</v>
+      </c>
+      <c r="E3" s="39" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="40" t="s">
-        <v>95</v>
-      </c>
-      <c r="B11" s="40"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="40"/>
+      <c r="A11" s="43" t="s">
+        <v>102</v>
+      </c>
+      <c r="B11" s="43"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="43"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C12" s="4"/>
@@ -3013,17 +3012,17 @@
       <c r="I12" s="5"/>
     </row>
     <row r="13" spans="1:9" ht="234" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="40" t="s">
-        <v>59</v>
-      </c>
-      <c r="B13" s="40"/>
-      <c r="C13" s="40"/>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="40"/>
+      <c r="A13" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" s="43"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="43"/>
+      <c r="I13" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -3059,7 +3058,7 @@
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>41</v>
       </c>
@@ -3080,35 +3079,35 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="120" x14ac:dyDescent="0.25">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="51" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="48"/>
-      <c r="C2" s="89" t="s">
-        <v>98</v>
-      </c>
-      <c r="D2" s="89" t="s">
-        <v>99</v>
-      </c>
-      <c r="E2" s="91" t="s">
-        <v>70</v>
-      </c>
-      <c r="F2" s="89" t="s">
-        <v>100</v>
+      <c r="B2" s="51"/>
+      <c r="C2" s="37" t="s">
+        <v>93</v>
+      </c>
+      <c r="D2" s="37" t="s">
+        <v>94</v>
+      </c>
+      <c r="E2" s="39" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" s="37" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="11" spans="1:9" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="40" t="s">
-        <v>97</v>
-      </c>
-      <c r="B11" s="40"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="40"/>
+      <c r="A11" s="43" t="s">
+        <v>92</v>
+      </c>
+      <c r="B11" s="43"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="43"/>
     </row>
     <row r="12" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
@@ -3122,17 +3121,17 @@
       <c r="I12" s="5"/>
     </row>
     <row r="13" spans="1:9" customFormat="1" ht="234" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="40" t="s">
-        <v>59</v>
-      </c>
-      <c r="B13" s="40"/>
-      <c r="C13" s="40"/>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="40"/>
+      <c r="A13" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" s="43"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="43"/>
+      <c r="I13" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3148,7 +3147,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
@@ -3161,20 +3160,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="81" t="s">
+      <c r="B1" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="85" t="s">
+      <c r="C1" s="90" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="86"/>
+      <c r="D1" s="91"/>
     </row>
     <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="47"/>
-      <c r="B2" s="82"/>
+      <c r="A2" s="50"/>
+      <c r="B2" s="87"/>
       <c r="C2" s="10" t="s">
         <v>21</v>
       </c>
@@ -3183,29 +3182,29 @@
       </c>
     </row>
     <row r="3" spans="1:14" ht="120" x14ac:dyDescent="0.25">
-      <c r="A3" s="87" t="s">
+      <c r="A3" s="72" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="88"/>
-      <c r="C3" s="89" t="s">
-        <v>101</v>
-      </c>
-      <c r="D3" s="89" t="s">
-        <v>102</v>
+      <c r="B3" s="73"/>
+      <c r="C3" s="37" t="s">
+        <v>96</v>
+      </c>
+      <c r="D3" s="37" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:14" s="7" customFormat="1" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="B11" s="40"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="40"/>
+      <c r="A11" s="43" t="s">
+        <v>100</v>
+      </c>
+      <c r="B11" s="43"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="43"/>
       <c r="J11" s="5"/>
       <c r="K11" s="4"/>
       <c r="L11" s="3"/>
@@ -3229,17 +3228,17 @@
       <c r="N12" s="5"/>
     </row>
     <row r="13" spans="1:14" s="7" customFormat="1" ht="225" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="40" t="s">
-        <v>59</v>
-      </c>
-      <c r="B13" s="40"/>
-      <c r="C13" s="40"/>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="40"/>
+      <c r="A13" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" s="43"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="43"/>
+      <c r="I13" s="43"/>
       <c r="J13" s="5"/>
       <c r="K13" s="4"/>
       <c r="L13" s="3"/>

</xml_diff>